<commit_message>
delete clock add /ping
</commit_message>
<xml_diff>
--- a/StockAPP/02-DataDesign/LandingFile.xlsx
+++ b/StockAPP/02-DataDesign/LandingFile.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/94980caa470a6302/文档/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\RunStockProject\StockAPP\02-DataDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CF589DD-48B2-4B41-9613-497546F5D868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D94BC8C6-C8BD-4D65-9DB5-CA77E5185B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="675" windowWidth="14243" windowHeight="9300" xr2:uid="{E951710A-EE1D-4094-95BC-67C0335A48B9}"/>
+    <workbookView xWindow="11820" yWindow="0" windowWidth="12951" windowHeight="14794" firstSheet="1" activeTab="3" xr2:uid="{33978538-6832-427C-8C9A-808203D2EB8D}"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="CB_PARAM" sheetId="1" r:id="rId1"/>
+    <sheet name="UserId" sheetId="2" r:id="rId2"/>
+    <sheet name="UserKey" sheetId="3" r:id="rId3"/>
+    <sheet name="工作表4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,9 +36,183 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+  <si>
+    <t>Group1</t>
+  </si>
+  <si>
+    <t>Group2</t>
+  </si>
+  <si>
+    <t>Value_C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value_I</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>Lst_Maint_User</t>
+  </si>
+  <si>
+    <t>Lst_Maint_Dt</t>
+  </si>
+  <si>
+    <t>欄位名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中文名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>資料型態</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>說明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否為PK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>integer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User_No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User_Nm</t>
+  </si>
+  <si>
+    <t>Regested_Fg</t>
+  </si>
+  <si>
+    <t>Create_Dt</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>中文名稱</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>欄位名稱</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>資料型態</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>是否為</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PK</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>說明</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User_Key</t>
+  </si>
+  <si>
+    <t>User_Id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Product_Key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -51,21 +228,70 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -74,8 +300,23 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -391,13 +632,344 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9007717F-E843-43E1-B81C-739F644046BE}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FE44D9-DB51-4DED-92D9-23224D2E8ED6}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.149999999999999" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.45" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="11.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.3046875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.23046875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC329DF2-46EE-411F-8E90-808DB207765E}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.75" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.23046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.53515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D17F5324-D1B9-4A9B-87E3-174DD9C09553}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.75" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="10.61328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F253AEC-F6EC-4E70-991B-922B16AC401B}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.75" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.23046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.3046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>